<commit_message>
Update of Budget from Salvatore D'Antonio <salvatore.dantonio@uniparthenope.it>
</commit_message>
<xml_diff>
--- a/Budget/WP effort.xlsx
+++ b/Budget/WP effort.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fetzer/GIT/christoffetzer/SecureContainerPilot/Budget/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SEP\github\SecureContainerPilot\Budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="27405" windowHeight="12795" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WP Table" sheetId="1" r:id="rId1"/>
     <sheet name="Other Costs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -210,7 +207,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
@@ -522,38 +519,41 @@
     </xf>
   </cellXfs>
   <cellStyles count="26">
-    <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -824,24 +824,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.375" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
     <col min="12" max="12" width="13.5" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" customWidth="1"/>
-    <col min="15" max="15" width="7.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13.625" customWidth="1"/>
+    <col min="14" max="14" width="14.625" customWidth="1"/>
+    <col min="15" max="15" width="7.875" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -889,7 +889,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
@@ -940,7 +940,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -991,7 +991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>40</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>39</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1166,14 +1166,14 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1247,7 +1247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
         <v>25</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
         <v>38</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J14" t="s">
         <v>28</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
         <v>30</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J16" s="4" t="s">
         <v>31</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>32</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>33</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
         <v>34</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
         <v>35</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
         <v>36</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M24" s="35" t="s">
         <v>0</v>
       </c>
@@ -1404,7 +1404,7 @@
       <c r="P24" s="37"/>
       <c r="Q24" s="37"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M25" s="8"/>
       <c r="N25" s="39" t="s">
         <v>55</v>
@@ -1419,7 +1419,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="27" t="s">
         <v>6</v>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="O26" s="45">
         <f>N26/$N$29</f>
-        <v>0.49796069707081941</v>
+        <v>0.49814540059347179</v>
       </c>
       <c r="P26" s="38">
         <f>B36</f>
@@ -1447,10 +1447,10 @@
       </c>
       <c r="Q26" s="12">
         <f>P26/$P$29</f>
-        <v>0.49796069707081941</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0.49814540059347179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>43</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>7000</v>
       </c>
       <c r="C27" s="30">
-        <v>7000</v>
+        <v>4500</v>
       </c>
       <c r="D27" s="29">
         <v>7000</v>
@@ -1468,22 +1468,22 @@
       </c>
       <c r="N27" s="36">
         <f>C35</f>
-        <v>846250</v>
+        <v>845000</v>
       </c>
       <c r="O27" s="45">
         <f t="shared" ref="O27:O28" si="3">N27/$N$29</f>
-        <v>0.25101965146459027</v>
+        <v>0.25074183976261127</v>
       </c>
       <c r="P27" s="38">
         <f>C36</f>
-        <v>592375</v>
+        <v>591500</v>
       </c>
       <c r="Q27" s="12">
         <f t="shared" ref="Q27:Q28" si="4">P27/$P$29</f>
-        <v>0.25101965146459027</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0.25074183976261127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>44</v>
       </c>
@@ -1492,8 +1492,7 @@
         <v>168</v>
       </c>
       <c r="C28" s="28">
-        <f>G3</f>
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="D28" s="27">
         <f>G4</f>
@@ -1508,7 +1507,7 @@
       </c>
       <c r="O28" s="45">
         <f t="shared" si="3"/>
-        <v>0.25101965146459027</v>
+        <v>0.25111275964391694</v>
       </c>
       <c r="P28" s="38">
         <f>D36</f>
@@ -1516,10 +1515,10 @@
       </c>
       <c r="Q28" s="12">
         <f t="shared" si="4"/>
-        <v>0.25101965146459027</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0.25111275964391694</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>45</v>
       </c>
@@ -1537,16 +1536,16 @@
       </c>
       <c r="N29" s="42">
         <f>SUM(N26:N28)</f>
-        <v>3371250</v>
+        <v>3370000</v>
       </c>
       <c r="O29" s="46"/>
       <c r="P29" s="43">
         <f>SUM(P26:P28)</f>
-        <v>2359875</v>
+        <v>2359000</v>
       </c>
       <c r="Q29" s="44"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>46</v>
       </c>
@@ -1556,14 +1555,14 @@
       </c>
       <c r="C30" s="30">
         <f>C27*SUM(C28,C29)</f>
-        <v>595000</v>
+        <v>594000</v>
       </c>
       <c r="D30" s="29">
         <f>D27*SUM(D28,D29)</f>
         <v>595000</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>52</v>
       </c>
@@ -1580,7 +1579,7 @@
         <v>82000</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
         <v>47</v>
       </c>
@@ -1594,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>48</v>
       </c>
@@ -1608,7 +1607,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>49</v>
       </c>
@@ -1618,14 +1617,14 @@
       </c>
       <c r="C34" s="30">
         <f t="shared" ref="C34:D34" si="5">C33*SUM(C30,C31)</f>
-        <v>169250</v>
+        <v>169000</v>
       </c>
       <c r="D34" s="29">
         <f t="shared" si="5"/>
         <v>169250</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
         <v>50</v>
       </c>
@@ -1635,14 +1634,14 @@
       </c>
       <c r="C35" s="30">
         <f t="shared" ref="C35:D35" si="6">SUM(C30,C31,C32,C34)</f>
-        <v>846250</v>
+        <v>845000</v>
       </c>
       <c r="D35" s="29">
         <f t="shared" si="6"/>
         <v>846250</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
         <v>51</v>
       </c>
@@ -1652,23 +1651,23 @@
       </c>
       <c r="C36" s="30">
         <f>0.7*C35</f>
-        <v>592375</v>
+        <v>591500</v>
       </c>
       <c r="D36" s="29">
         <f>0.7*D35</f>
         <v>592375</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>58</v>
       </c>
       <c r="B38" s="34">
         <f>SUM(B35:D35)</f>
-        <v>3371250</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3370000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>57</v>
       </c>
@@ -1677,13 +1676,13 @@
         <v>331000</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="13">
         <f>B39/B38</f>
-        <v>9.8183166481275494E-2</v>
+        <v>9.821958456973294E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1699,14 +1698,14 @@
       <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.625" customWidth="1"/>
     <col min="2" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" customWidth="1"/>
+    <col min="5" max="5" width="30.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -1727,7 +1726,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -1744,7 +1743,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1761,7 +1760,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1778,7 +1777,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1789,7 +1788,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -1820,7 +1819,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1834,7 +1833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1848,7 +1847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1862,7 +1861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1876,7 +1875,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>

</xml_diff>